<commit_message>
med + butter filter
</commit_message>
<xml_diff>
--- a/notebooks/test_output/cv_results_no_load.xlsx
+++ b/notebooks/test_output/cv_results_no_load.xlsx
@@ -481,113 +481,113 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>30hz</t>
+          <t>10hz</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.96875</v>
+        <v>0.83125</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03423265984407288</v>
+        <v>0.04238956239453293</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.90625</v>
       </c>
       <c r="E2" t="n">
-        <v>0.90625</v>
+        <v>0.78125</v>
       </c>
       <c r="F2" t="n">
-        <v>28.29899053776933</v>
+        <v>19.60977554251545</v>
       </c>
       <c r="G2" t="n">
         <v>160</v>
       </c>
       <c r="H2" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20hz</t>
+          <t>30hz</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.95625</v>
+        <v>0.825</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0375</v>
+        <v>0.025</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="E3" t="n">
-        <v>0.90625</v>
+        <v>0.8125</v>
       </c>
       <c r="F3" t="n">
-        <v>25.49999320000181</v>
+        <v>32.99998680000527</v>
       </c>
       <c r="G3" t="n">
         <v>160</v>
       </c>
       <c r="H3" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10hz</t>
+          <t>40hz</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.94375</v>
+        <v>0.7875</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05</v>
+        <v>0.0125</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0.8125</v>
       </c>
       <c r="E4" t="n">
-        <v>0.875</v>
+        <v>0.78125</v>
       </c>
       <c r="F4" t="n">
-        <v>18.87499622500076</v>
+        <v>62.99994960004032</v>
       </c>
       <c r="G4" t="n">
         <v>160</v>
       </c>
       <c r="H4" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>40hz</t>
+          <t>20hz</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.91875</v>
+        <v>0.75</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05796011559684815</v>
+        <v>0.0625</v>
       </c>
       <c r="D5" t="n">
-        <v>0.96875</v>
+        <v>0.875</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8125</v>
+        <v>0.71875</v>
       </c>
       <c r="F5" t="n">
-        <v>15.8514149260222</v>
+        <v>11.99999808000031</v>
       </c>
       <c r="G5" t="n">
         <v>160</v>
       </c>
       <c r="H5" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9375</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="3">
@@ -649,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="4">
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.875</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="5">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="6">
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.90625</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="7">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="8">
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9375</v>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="9">
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="10">
@@ -740,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>0.90625</v>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="11">
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9375</v>
+        <v>0.71875</v>
       </c>
     </row>
     <row r="12">
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="13">
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>0.96875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="14">
@@ -792,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>0.96875</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="15">
@@ -805,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>0.90625</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="16">
@@ -818,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="17">
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.90625</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="18">
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>0.96875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="19">
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="20">
@@ -870,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>0.96875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="21">
@@ -883,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8125</v>
+        <v>0.78125</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30hz</t>
+          <t>10hz</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>40hz</t>
+          <t>20hz</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>30hz</t>
+          <t>40hz</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-02 16:36:44</t>
+          <t>2025-10-02 20:31:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
band freq domain features upd
</commit_message>
<xml_diff>
--- a/notebooks/test_output/cv_results_no_load.xlsx
+++ b/notebooks/test_output/cv_results_no_load.xlsx
@@ -481,113 +481,113 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10hz</t>
+          <t>30hz</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.83125</v>
+        <v>0.9375</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04238956239453293</v>
+        <v>0.05929270612815711</v>
       </c>
       <c r="D2" t="n">
-        <v>0.90625</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.78125</v>
+        <v>0.84375</v>
       </c>
       <c r="F2" t="n">
-        <v>19.60977554251545</v>
+        <v>15.81138563417568</v>
       </c>
       <c r="G2" t="n">
         <v>160</v>
       </c>
       <c r="H2" t="n">
-        <v>89</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>30hz</t>
+          <t>10hz</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.825</v>
+        <v>0.93125</v>
       </c>
       <c r="C3" t="n">
-        <v>0.025</v>
+        <v>0.02338535866733714</v>
       </c>
       <c r="D3" t="n">
-        <v>0.875</v>
+        <v>0.96875</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8125</v>
+        <v>0.90625</v>
       </c>
       <c r="F3" t="n">
-        <v>32.99998680000527</v>
+        <v>39.82190801638708</v>
       </c>
       <c r="G3" t="n">
         <v>160</v>
       </c>
       <c r="H3" t="n">
-        <v>90</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>40hz</t>
+          <t>20hz</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7875</v>
+        <v>0.8875</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0125</v>
+        <v>0.0318688719599549</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8125</v>
+        <v>0.9375</v>
       </c>
       <c r="E4" t="n">
-        <v>0.78125</v>
+        <v>0.84375</v>
       </c>
       <c r="F4" t="n">
-        <v>62.99994960004032</v>
+        <v>27.84848245116334</v>
       </c>
       <c r="G4" t="n">
         <v>160</v>
       </c>
       <c r="H4" t="n">
-        <v>89</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20hz</t>
+          <t>40hz</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0625</v>
+        <v>0.05590169943749474</v>
       </c>
       <c r="D5" t="n">
-        <v>0.875</v>
+        <v>0.9375</v>
       </c>
       <c r="E5" t="n">
-        <v>0.71875</v>
+        <v>0.78125</v>
       </c>
       <c r="F5" t="n">
-        <v>11.99999808000031</v>
+        <v>15.65247304249903</v>
       </c>
       <c r="G5" t="n">
         <v>160</v>
       </c>
       <c r="H5" t="n">
-        <v>89</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.90625</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="3">
@@ -649,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.78125</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="4">
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.84375</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="5">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8125</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="6">
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8125</v>
+        <v>0.96875</v>
       </c>
     </row>
     <row r="7">
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.71875</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="8">
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.71875</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="9">
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0.875</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="10">
@@ -740,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>0.71875</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="11">
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.71875</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="12">
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8125</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="14">
@@ -792,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -805,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8125</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="16">
@@ -818,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.875</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="17">
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.78125</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="18">
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8125</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="20">
@@ -870,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>0.78125</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="21">
@@ -883,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.78125</v>
+        <v>0.90625</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10hz</t>
+          <t>30hz</t>
         </is>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>20hz</t>
+          <t>40hz</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>40hz</t>
+          <t>10hz</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-02 20:31:00</t>
+          <t>2025-10-03 16:22:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
features edit, features crosscor
</commit_message>
<xml_diff>
--- a/notebooks/test_output/cv_results_no_load.xlsx
+++ b/notebooks/test_output/cv_results_no_load.xlsx
@@ -485,109 +485,109 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9375</v>
+        <v>0.921875</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05929270612815711</v>
+        <v>0.0369754986443726</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.96875</v>
       </c>
       <c r="E2" t="n">
-        <v>0.84375</v>
+        <v>0.859375</v>
       </c>
       <c r="F2" t="n">
-        <v>15.81138563417568</v>
+        <v>24.93204377163592</v>
       </c>
       <c r="G2" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="H2" t="n">
-        <v>246</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10hz</t>
+          <t>40hz</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.93125</v>
+        <v>0.88125</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02338535866733714</v>
+        <v>0.04485218779502289</v>
       </c>
       <c r="D3" t="n">
-        <v>0.96875</v>
+        <v>0.9375</v>
       </c>
       <c r="E3" t="n">
-        <v>0.90625</v>
+        <v>0.8125</v>
       </c>
       <c r="F3" t="n">
-        <v>39.82190801638708</v>
+        <v>19.64786662244207</v>
       </c>
       <c r="G3" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="H3" t="n">
-        <v>246</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20hz</t>
+          <t>10hz</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8875</v>
+        <v>0.86875</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0318688719599549</v>
+        <v>0.02538762001448738</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9375</v>
+        <v>0.90625</v>
       </c>
       <c r="E4" t="n">
         <v>0.84375</v>
       </c>
       <c r="F4" t="n">
-        <v>27.84848245116334</v>
+        <v>34.21942101347193</v>
       </c>
       <c r="G4" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="H4" t="n">
-        <v>246</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>40hz</t>
+          <t>20hz</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.875</v>
+        <v>0.853125</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05590169943749474</v>
+        <v>0.03365728004459066</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9375</v>
+        <v>0.890625</v>
       </c>
       <c r="E5" t="n">
-        <v>0.78125</v>
+        <v>0.8125</v>
       </c>
       <c r="F5" t="n">
-        <v>15.65247304249903</v>
+        <v>25.34740613013533</v>
       </c>
       <c r="G5" t="n">
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="H5" t="n">
-        <v>246</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9375</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="3">
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.90625</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="5">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9375</v>
+        <v>0.890625</v>
       </c>
     </row>
     <row r="6">
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>0.96875</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="7">
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="9">
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0.90625</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="10">
@@ -740,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>0.875</v>
+        <v>0.890625</v>
       </c>
     </row>
     <row r="11">
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>0.84375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="12">
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0.96875</v>
       </c>
     </row>
     <row r="13">
@@ -792,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="15">
@@ -805,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>0.90625</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="16">
@@ -818,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.84375</v>
+        <v>0.90625</v>
       </c>
     </row>
     <row r="17">
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>0.90625</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="18">
@@ -844,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>0.78125</v>
+        <v>0.921875</v>
       </c>
     </row>
     <row r="19">
@@ -857,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>0.84375</v>
+        <v>0.859375</v>
       </c>
     </row>
     <row r="20">
@@ -870,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9375</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="21">
@@ -883,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.90625</v>
+        <v>0.9375</v>
       </c>
     </row>
   </sheetData>
@@ -937,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D2" t="n">
         <v>25</v>
@@ -953,7 +953,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D3" t="n">
         <v>25</v>
@@ -969,7 +969,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D4" t="n">
         <v>25</v>
@@ -985,7 +985,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D5" t="n">
         <v>25</v>
@@ -1001,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D6" t="n">
         <v>25</v>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D7" t="n">
         <v>25</v>
@@ -1033,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D8" t="n">
         <v>25</v>
@@ -1049,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D9" t="n">
         <v>25</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D10" t="n">
         <v>25</v>
@@ -1081,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D11" t="n">
         <v>25</v>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D12" t="n">
         <v>25</v>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D13" t="n">
         <v>25</v>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D14" t="n">
         <v>25</v>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D15" t="n">
         <v>25</v>
@@ -1161,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D16" t="n">
         <v>25</v>
@@ -1177,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D17" t="n">
         <v>25</v>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>40hz</t>
+          <t>20hz</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-03 16:22:27</t>
+          <t>2025-10-06 15:13:44</t>
         </is>
       </c>
     </row>

</xml_diff>